<commit_message>
trying zeroshot training now. sample 5000, zeroshot minsim 0.7.
</commit_message>
<xml_diff>
--- a/model_tests.xlsx
+++ b/model_tests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cd5619e07473d5e8/Dokumente/winfoMaster/Masterarbeit/bertopic_ecc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="11_AD4DB114E441178AC67DF4A9A614CC6A693EDF1B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{606CE1F9-7C51-4C95-8B95-C83B4E6DFC8B}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="11_AD4DB114E441178AC67DF4A9A614CC6A693EDF1B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{56A38639-3C70-404D-8BC6-37E9AB9CBF32}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Model</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>bertopic_model_dir_regular_5_50_finbert_local</t>
+  </si>
+  <si>
+    <t>ncomp</t>
   </si>
 </sst>
 </file>
@@ -366,18 +369,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C3:F7"/>
+  <dimension ref="C3:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="44.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>0</v>
       </c>
@@ -388,10 +391,13 @@
         <v>4</v>
       </c>
       <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>2</v>
       </c>
@@ -401,22 +407,22 @@
       <c r="E4">
         <v>60</v>
       </c>
-      <c r="F4">
+      <c r="H4">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>3</v>
       </c>
       <c r="D5">
         <v>20</v>
       </c>
-      <c r="F5">
+      <c r="H5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>6</v>
       </c>
@@ -426,11 +432,11 @@
       <c r="E6">
         <v>60</v>
       </c>
-      <c r="F6">
+      <c r="H6">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>7</v>
       </c>
@@ -440,7 +446,7 @@
       <c r="E7">
         <v>50</v>
       </c>
-      <c r="F7">
+      <c r="H7">
         <v>5</v>
       </c>
     </row>

</xml_diff>